<commit_message>
worked on arithmetic unit
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E3AB59-284D-4716-8A26-CC5FFA9DFD14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DEC8F6-05FE-4A0D-BFD2-BDD59D268FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11835" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log" sheetId="1" r:id="rId1"/>
@@ -74,22 +74,22 @@
     <t>29/03/2020</t>
   </si>
   <si>
-    <t>9:20pm</t>
-  </si>
-  <si>
     <t>Started reading about the implementation of Arithmetic Unit</t>
   </si>
   <si>
-    <t>9:50pm</t>
+    <t>Setup modelsim</t>
   </si>
   <si>
-    <t>9:55pm</t>
+    <t>30/03/2020</t>
   </si>
   <si>
-    <t>10:45pm</t>
+    <t>31/03/2020</t>
   </si>
   <si>
-    <t>Setup modelsim</t>
+    <t>Completed full adder and ripple adder</t>
+  </si>
+  <si>
+    <t>Finished Arithmetic unit</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
   <dimension ref="A1:G756"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,14 +746,14 @@
       <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="18">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E6" s="21">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -763,29 +763,49 @@
       <c r="C7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="19">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="E7" s="22">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="19">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="13" t="s">
+      <c r="D9" s="19">
+        <v>0.8618055555555556</v>
+      </c>
+      <c r="E9" s="22">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="G9" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="22"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="22"/>
-      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13"/>

</xml_diff>

<commit_message>
added screenshots and documentation
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DEC8F6-05FE-4A0D-BFD2-BDD59D268FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADCF9BE-5D3A-4DAC-B148-6BE61E3E7E8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -90,6 +90,21 @@
   </si>
   <si>
     <t>Finished Arithmetic unit</t>
+  </si>
+  <si>
+    <t>01/04/2020</t>
+  </si>
+  <si>
+    <t>Help debug arithmetic unit</t>
+  </si>
+  <si>
+    <t>02/04/2020</t>
+  </si>
+  <si>
+    <t>Screenshots of functional simulation waves</t>
+  </si>
+  <si>
+    <t>Working on documentations and project report</t>
   </si>
 </sst>
 </file>
@@ -676,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G756"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,25 +823,51 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="22"/>
-      <c r="G10" s="13"/>
+      <c r="B10" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.625</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0.68194444444444446</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E11" s="22">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="19">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="E12" s="22">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>

</xml_diff>

<commit_message>
adding screenshots on documentations
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DEC8F6-05FE-4A0D-BFD2-BDD59D268FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602A73E9-B3D7-4385-B4C6-3B9249E20071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -89,7 +89,22 @@
     <t>Completed full adder and ripple adder</t>
   </si>
   <si>
-    <t>Finished Arithmetic unit</t>
+    <t>01/04/2020</t>
+  </si>
+  <si>
+    <t>Help debug arithmetic unit</t>
+  </si>
+  <si>
+    <t>worked Arithmetic unit</t>
+  </si>
+  <si>
+    <t>02/04/2020</t>
+  </si>
+  <si>
+    <t>Screenshots of waves of functional simulation</t>
+  </si>
+  <si>
+    <t>Worked on documentations</t>
   </si>
 </sst>
 </file>
@@ -676,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G756"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,29 +819,55 @@
         <v>0.43055555555555558</v>
       </c>
       <c r="G9" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="22"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="19">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E11" s="22">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="19">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="E12" s="22">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>

</xml_diff>

<commit_message>
Update logs changing into subtasks
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602A73E9-B3D7-4385-B4C6-3B9249E20071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BC1050-9E00-4D2E-9F60-F629B64EDDC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -71,40 +71,37 @@
     <t>Group Number: 54</t>
   </si>
   <si>
-    <t>29/03/2020</t>
-  </si>
-  <si>
     <t>Started reading about the implementation of Arithmetic Unit</t>
-  </si>
-  <si>
-    <t>Setup modelsim</t>
-  </si>
-  <si>
-    <t>30/03/2020</t>
-  </si>
-  <si>
-    <t>31/03/2020</t>
-  </si>
-  <si>
-    <t>Completed full adder and ripple adder</t>
-  </si>
-  <si>
-    <t>01/04/2020</t>
   </si>
   <si>
     <t>Help debug arithmetic unit</t>
   </si>
   <si>
-    <t>worked Arithmetic unit</t>
-  </si>
-  <si>
-    <t>02/04/2020</t>
-  </si>
-  <si>
     <t>Screenshots of waves of functional simulation</t>
   </si>
   <si>
-    <t>Worked on documentations</t>
+    <t>Writing up report and proofreading</t>
+  </si>
+  <si>
+    <t>Cleaning up documentations and finishing up</t>
+  </si>
+  <si>
+    <t>Setting up work environment, git and modelsim</t>
+  </si>
+  <si>
+    <t>Worked on arithmetic unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on ripple adder </t>
+  </si>
+  <si>
+    <t>Worked on full adder</t>
+  </si>
+  <si>
+    <t>Helping with screenshots of timing simulations</t>
+  </si>
+  <si>
+    <t>Start working on documentations, screenshot descriptions, etc.</t>
   </si>
 </sst>
 </file>
@@ -691,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G756"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,8 +755,8 @@
       <c r="B6" s="12">
         <v>4794</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>9</v>
+      <c r="C6" s="9">
+        <v>43919</v>
       </c>
       <c r="D6" s="18">
         <v>0.88888888888888884</v>
@@ -768,15 +765,15 @@
         <v>0.90972222222222221</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13">
         <v>4794</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>9</v>
+      <c r="C7" s="10">
+        <v>43919</v>
       </c>
       <c r="D7" s="19">
         <v>0.91319444444444453</v>
@@ -785,117 +782,161 @@
         <v>0.94791666666666663</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13">
         <v>4794</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>12</v>
+      <c r="C8" s="10">
+        <v>43920</v>
       </c>
       <c r="D8" s="19">
         <v>0.86805555555555547</v>
       </c>
       <c r="E8" s="22">
-        <v>0.95138888888888884</v>
+        <v>0.90625</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
         <v>4794</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>13</v>
+      <c r="C9" s="10">
+        <v>43920</v>
       </c>
       <c r="D9" s="19">
-        <v>0.8618055555555556</v>
+        <v>0.90625</v>
       </c>
       <c r="E9" s="22">
-        <v>0.43055555555555558</v>
+        <v>0.95138888888888884</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <v>4794</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="10">
+        <v>43921</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="19">
+    </row>
+    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C11" s="10">
+        <v>43922</v>
+      </c>
+      <c r="D11" s="19">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E11" s="22">
         <v>0.66666666666666663</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
-      <c r="C11" s="10" t="s">
+      <c r="G11" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C12" s="10">
+        <v>43923</v>
+      </c>
+      <c r="D12" s="19">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E12" s="22">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C13" s="10">
+        <v>43923</v>
+      </c>
+      <c r="D13" s="19">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="E13" s="22">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="19">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="E11" s="22">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="G11" s="13" t="s">
+    </row>
+    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C14" s="10">
+        <v>43923</v>
+      </c>
+      <c r="D14" s="19">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="E14" s="22">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="19">
-        <v>0.81944444444444453</v>
-      </c>
-      <c r="E12" s="22">
-        <v>0.94791666666666663</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="22"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="22"/>
-      <c r="G14" s="13"/>
-    </row>
     <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="22"/>
-      <c r="G15" s="13"/>
+      <c r="B15" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C15" s="10">
+        <v>43924</v>
+      </c>
+      <c r="D15" s="19">
+        <v>0.71875</v>
+      </c>
+      <c r="E15" s="22">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="22"/>
-      <c r="G16" s="13"/>
+      <c r="B16" s="13">
+        <v>4794</v>
+      </c>
+      <c r="C16" s="10">
+        <v>43926</v>
+      </c>
+      <c r="D16" s="19">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="E16" s="22">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
@@ -1144,13 +1185,23 @@
     </row>
     <row r="52" spans="2:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="14"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="23"/>
-      <c r="G52" s="14"/>
-    </row>
-    <row r="53" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="22"/>
+      <c r="G52" s="13"/>
+    </row>
+    <row r="53" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="10"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="22"/>
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="2:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="11"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="23"/>
+      <c r="G54" s="14"/>
+    </row>
     <row r="55" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Final update to logs
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-4794-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BC1050-9E00-4D2E-9F60-F629B64EDDC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFC0205-6E62-4755-9589-6D5FD279C51D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Started reading about the implementation of Arithmetic Unit</t>
   </si>
   <si>
-    <t>Help debug arithmetic unit</t>
-  </si>
-  <si>
     <t>Screenshots of waves of functional simulation</t>
   </si>
   <si>
@@ -89,19 +86,25 @@
     <t>Setting up work environment, git and modelsim</t>
   </si>
   <si>
-    <t>Worked on arithmetic unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Worked on ripple adder </t>
-  </si>
-  <si>
-    <t>Worked on full adder</t>
-  </si>
-  <si>
     <t>Helping with screenshots of timing simulations</t>
   </si>
   <si>
     <t>Start working on documentations, screenshot descriptions, etc.</t>
+  </si>
+  <si>
+    <t>Adding anotations to pdf and submitting</t>
+  </si>
+  <si>
+    <t>Worked on arithmetic unit implementing Adder, Zero, ExtWord MUX, AltB  and AltBu</t>
+  </si>
+  <si>
+    <t>Help debug arithmetic unit (errors with sign extension) Output ExtWord was not matching with test bench values</t>
+  </si>
+  <si>
+    <t>Worked on full adder implementation</t>
+  </si>
+  <si>
+    <t>Worked on ripple adder implementation</t>
   </si>
 </sst>
 </file>
@@ -688,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G756"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +785,7 @@
         <v>0.94791666666666663</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -799,7 +802,7 @@
         <v>0.90625</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -816,7 +819,7 @@
         <v>0.95138888888888884</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -833,7 +836,7 @@
         <v>0.93055555555555547</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -850,7 +853,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -867,7 +870,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -884,7 +887,7 @@
         <v>0.86458333333333337</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -901,7 +904,7 @@
         <v>0.94791666666666663</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -918,7 +921,7 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -932,18 +935,26 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="E16" s="22">
-        <v>0.64583333333333337</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="22"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="10">
+        <v>43926</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E17" s="22">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13"/>

</xml_diff>